<commit_message>
Ready to branch to Master
</commit_message>
<xml_diff>
--- a/Excel/Production_estimator.xlsx
+++ b/Excel/Production_estimator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anaconda\Documents\Node_JS\Intro_Software\REACT_Native\Sandvik\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16017773-9CF8-4847-AD1B-A79B3118FBD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391ED4FE-94C0-43BC-9110-2CEF02B0EF6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4824" yWindow="324" windowWidth="10368" windowHeight="5952" xr2:uid="{1E8DBCC9-7E63-45D7-8A1F-24A422C36920}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1E8DBCC9-7E63-45D7-8A1F-24A422C36920}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -4616,7 +4616,7 @@
   <dimension ref="A1:AD37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5047,7 +5047,7 @@
       <c r="G10" s="83"/>
       <c r="H10" s="70">
         <f>L10/D11</f>
-        <v>787.89814814814804</v>
+        <v>451.60998961297031</v>
       </c>
       <c r="I10" s="8">
         <f>J10*K10</f>
@@ -5061,7 +5061,7 @@
       </c>
       <c r="L10" s="8">
         <f>D12</f>
-        <v>872321.43472222204</v>
+        <v>500000</v>
       </c>
       <c r="M10" s="10">
         <v>1</v>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="M11" s="15">
         <f>L11/$L$10</f>
-        <v>1.0563682730018389</v>
+        <v>1.842985375</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -5150,8 +5150,7 @@
       </c>
       <c r="C12" s="84"/>
       <c r="D12" s="77">
-        <f>E15</f>
-        <v>872321.43472222204</v>
+        <v>500000</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="83" t="s">
@@ -5180,7 +5179,7 @@
       </c>
       <c r="M12" s="15">
         <f>L12/$L$10</f>
-        <v>1.0585241266202097</v>
+        <v>1.8467465696428567</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>119</v>
@@ -5238,7 +5237,7 @@
       </c>
       <c r="M13" s="15">
         <f>L13/$L$10</f>
-        <v>1.1643765392822307</v>
+        <v>2.0314212266071423</v>
       </c>
       <c r="N13" s="80">
         <f>'Water Fall Info'!N13</f>
@@ -5301,7 +5300,7 @@
       </c>
       <c r="M14" s="15">
         <f>L14/$L$10</f>
-        <v>1.2209706547961807</v>
+        <v>2.1301577466910704</v>
       </c>
       <c r="N14" s="80">
         <f>'Water Fall Info'!I33</f>
@@ -6931,7 +6930,7 @@
       </c>
       <c r="F31" s="26">
         <f>Summary!D12/'Water Fall Info'!B12</f>
-        <v>14339.530433789951</v>
+        <v>8219.17808219178</v>
       </c>
       <c r="G31" s="56">
         <f>G22*Summary!D10</f>
@@ -7161,21 +7160,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B213CCA8013F15498614EFF528826B54" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a91674ab2ffb5a13b82b9dc442c7dea6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="589a4ccc-1179-4918-b5a3-df951319a05f" xmlns:ns4="5a2f2624-f98c-49c1-96fa-2e7f7a2b0df6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3a16099a1832cbda7f407950f0eef236" ns3:_="" ns4:_="">
     <xsd:import namespace="589a4ccc-1179-4918-b5a3-df951319a05f"/>
@@ -7398,32 +7382,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC85043C-4ED8-4A3E-80F2-A3023AE56E51}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="589a4ccc-1179-4918-b5a3-df951319a05f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="5a2f2624-f98c-49c1-96fa-2e7f7a2b0df6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B75507E-D178-4B48-90CB-ECAE3FB6F66D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92953386-EC89-415A-B75F-2AFFEEE59D3C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7440,4 +7414,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B75507E-D178-4B48-90CB-ECAE3FB6F66D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC85043C-4ED8-4A3E-80F2-A3023AE56E51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="589a4ccc-1179-4918-b5a3-df951319a05f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="5a2f2624-f98c-49c1-96fa-2e7f7a2b0df6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>